<commit_message>
Perbaikan seeder dan kolom nidn dosen
</commit_message>
<xml_diff>
--- a/public/import_seed/dosen_2019.xlsx
+++ b/public/import_seed/dosen_2019.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="96">
   <si>
     <t>No</t>
   </si>
@@ -223,14 +223,99 @@
   </si>
   <si>
     <t>Pend. Teknologi Informasi</t>
+  </si>
+  <si>
+    <t>0028057802</t>
+  </si>
+  <si>
+    <t>197805282003122000</t>
+  </si>
+  <si>
+    <t>Sitti Suhada, S.Kom, MT</t>
+  </si>
+  <si>
+    <t>Moh. Ramdhan Arif Kaluku, S.Kom., M.Kom</t>
+  </si>
+  <si>
+    <t>0007048902</t>
+  </si>
+  <si>
+    <t>198904072015041004</t>
+  </si>
+  <si>
+    <t>Laki-Laki</t>
+  </si>
+  <si>
+    <t>Islam</t>
+  </si>
+  <si>
+    <t>0002017206</t>
+  </si>
+  <si>
+    <t>00110585</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 00111291</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0014028602</t>
+  </si>
+  <si>
+    <t>00140387</t>
+  </si>
+  <si>
+    <t>0016047303</t>
+  </si>
+  <si>
+    <t>0017048001</t>
+  </si>
+  <si>
+    <t>0017087402</t>
+  </si>
+  <si>
+    <t>0020059003</t>
+  </si>
+  <si>
+    <t>0020078303</t>
+  </si>
+  <si>
+    <t>00210490</t>
+  </si>
+  <si>
+    <t>00221184</t>
+  </si>
+  <si>
+    <t>0025078202</t>
+  </si>
+  <si>
+    <t>0026056602</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0926058901</t>
+  </si>
+  <si>
+    <t>0928028101</t>
+  </si>
+  <si>
+    <t>0929048102</t>
+  </si>
+  <si>
+    <t>9900993739</t>
+  </si>
+  <si>
+    <t>00111192</t>
+  </si>
+  <si>
+    <t>00200393</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -281,7 +366,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -292,6 +377,9 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -599,8 +687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,7 +696,7 @@
     <col min="1" max="1" width="3.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50.85546875" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" customWidth="1"/>
+    <col min="4" max="4" width="29.5703125" customWidth="1"/>
     <col min="5" max="5" width="30.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.140625" bestFit="1" customWidth="1"/>
@@ -688,8 +776,8 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="5">
-        <v>2017206</v>
+      <c r="B2" s="8" t="s">
+        <v>76</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>28</v>
@@ -731,8 +819,8 @@
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="5">
-        <v>110585</v>
+      <c r="B3" s="8" t="s">
+        <v>77</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>29</v>
@@ -772,8 +860,8 @@
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="5">
-        <v>111291</v>
+      <c r="B4" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>30</v>
@@ -813,8 +901,8 @@
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="5">
-        <v>14028602</v>
+      <c r="B5" s="8" t="s">
+        <v>79</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>31</v>
@@ -856,8 +944,8 @@
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="5">
-        <v>140387</v>
+      <c r="B6" s="8" t="s">
+        <v>80</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>32</v>
@@ -897,8 +985,8 @@
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="5">
-        <v>16047303</v>
+      <c r="B7" s="8" t="s">
+        <v>81</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>33</v>
@@ -940,8 +1028,8 @@
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="5">
-        <v>17048001</v>
+      <c r="B8" s="8" t="s">
+        <v>82</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>34</v>
@@ -983,8 +1071,8 @@
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="5">
-        <v>17087402</v>
+      <c r="B9" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>35</v>
@@ -1026,8 +1114,8 @@
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="5">
-        <v>20059003</v>
+      <c r="B10" s="8" t="s">
+        <v>84</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>36</v>
@@ -1069,8 +1157,8 @@
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="5">
-        <v>20078303</v>
+      <c r="B11" s="8" t="s">
+        <v>85</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>37</v>
@@ -1112,8 +1200,8 @@
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="5">
-        <v>210490</v>
+      <c r="B12" s="8" t="s">
+        <v>86</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>38</v>
@@ -1153,8 +1241,8 @@
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="5">
-        <v>221184</v>
+      <c r="B13" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>39</v>
@@ -1194,8 +1282,8 @@
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="5">
-        <v>25078202</v>
+      <c r="B14" s="8" t="s">
+        <v>88</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>40</v>
@@ -1237,8 +1325,8 @@
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="5">
-        <v>26056602</v>
+      <c r="B15" s="8" t="s">
+        <v>89</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>41</v>
@@ -1280,8 +1368,8 @@
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="5">
-        <v>926058901</v>
+      <c r="B16" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>42</v>
@@ -1323,8 +1411,8 @@
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="5">
-        <v>928028101</v>
+      <c r="B17" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>43</v>
@@ -1364,8 +1452,8 @@
       <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="5">
-        <v>929048102</v>
+      <c r="B18" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>44</v>
@@ -1405,8 +1493,8 @@
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="5">
-        <v>9900993739</v>
+      <c r="B19" s="8" t="s">
+        <v>93</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>45</v>
@@ -1446,8 +1534,8 @@
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="5">
-        <v>111192</v>
+      <c r="B20" s="8" t="s">
+        <v>94</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>46</v>
@@ -1487,8 +1575,8 @@
       <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="5">
-        <v>200393</v>
+      <c r="B21" s="8" t="s">
+        <v>95</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>47</v>
@@ -1525,45 +1613,93 @@
       <c r="S21" s="1"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I22" s="10">
+        <v>28638</v>
+      </c>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
+      <c r="M22" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
-      <c r="Q22" s="1"/>
-      <c r="R22" s="1"/>
+      <c r="Q22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R22" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="S22" s="1"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I23" s="10">
+        <v>32605</v>
+      </c>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
+      <c r="M23" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
-      <c r="Q23" s="1"/>
-      <c r="R23" s="1"/>
+      <c r="Q23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R23" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="S23" s="1"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Penyesuaian ulang teknik penghitungan simulasi akreditasi
</commit_message>
<xml_diff>
--- a/public/import_seed/dosen_2019.xlsx
+++ b/public/import_seed/dosen_2019.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="95">
   <si>
     <t>No</t>
   </si>
@@ -205,9 +205,6 @@
   </si>
   <si>
     <t>SEMARANG</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1981-02-28</t>
   </si>
   <si>
     <t>Dosen SP Rumah Sakit</t>
@@ -313,9 +310,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -379,7 +375,7 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -688,7 +684,7 @@
   <dimension ref="A1:S51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,7 +773,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>28</v>
@@ -786,7 +782,7 @@
         <v>48</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>25</v>
@@ -820,17 +816,17 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>29</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="5" t="s">
@@ -849,7 +845,7 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="R3" s="5" t="s">
         <v>21</v>
@@ -861,14 +857,14 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>30</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>25</v>
@@ -902,7 +898,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>31</v>
@@ -911,7 +907,7 @@
         <v>49</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>25</v>
@@ -945,17 +941,17 @@
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>32</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="5" t="s">
@@ -974,7 +970,7 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R6" s="5" t="s">
         <v>21</v>
@@ -986,7 +982,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>33</v>
@@ -995,10 +991,10 @@
         <v>50</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="5" t="s">
@@ -1029,7 +1025,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>34</v>
@@ -1038,7 +1034,7 @@
         <v>51</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>25</v>
@@ -1072,7 +1068,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>35</v>
@@ -1081,10 +1077,10 @@
         <v>52</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="5" t="s">
@@ -1115,7 +1111,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>36</v>
@@ -1124,10 +1120,10 @@
         <v>53</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="5" t="s">
@@ -1146,7 +1142,7 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="R10" s="5" t="s">
         <v>21</v>
@@ -1158,7 +1154,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>37</v>
@@ -1167,10 +1163,10 @@
         <v>54</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="5" t="s">
@@ -1201,17 +1197,17 @@
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>38</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="5" t="s">
@@ -1230,7 +1226,7 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="R12" s="5" t="s">
         <v>21</v>
@@ -1242,17 +1238,17 @@
         <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>39</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="4" t="s">
@@ -1283,7 +1279,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>40</v>
@@ -1292,10 +1288,10 @@
         <v>55</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="4" t="s">
@@ -1326,7 +1322,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>41</v>
@@ -1335,10 +1331,10 @@
         <v>56</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="5" t="s">
@@ -1369,7 +1365,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>42</v>
@@ -1378,10 +1374,10 @@
         <v>57</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="5" t="s">
@@ -1412,24 +1408,24 @@
         <v>16</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>43</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="I17" s="7" t="s">
-        <v>62</v>
+      <c r="I17" s="7">
+        <v>29645</v>
       </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -1441,7 +1437,7 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R17" s="5" t="s">
         <v>21</v>
@@ -1453,17 +1449,17 @@
         <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>44</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="5" t="s">
@@ -1482,7 +1478,7 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R18" s="5" t="s">
         <v>21</v>
@@ -1494,14 +1490,14 @@
         <v>18</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>45</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>25</v>
@@ -1535,17 +1531,17 @@
         <v>19</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>46</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="5" t="s">
@@ -1576,17 +1572,17 @@
         <v>20</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="5" t="s">
@@ -1617,22 +1613,22 @@
         <v>21</v>
       </c>
       <c r="B22" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>69</v>
-      </c>
       <c r="E22" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>25</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>58</v>
@@ -1662,22 +1658,22 @@
         <v>22</v>
       </c>
       <c r="B23" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D23" s="9" t="s">
+      <c r="E23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F23" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>58</v>

</xml_diff>